<commit_message>
clarify other phytos in crosswalk/script
</commit_message>
<xml_diff>
--- a/Data/crosswalk.xlsx
+++ b/Data/crosswalk.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Labou\LTER_FA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Labou\LTER_FA\fa\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8256"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8256" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="LTER" sheetId="2" r:id="rId1"/>
+    <sheet name="EULI" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="35">
   <si>
     <t>"Cyanobacteria"</t>
   </si>
@@ -114,6 +115,21 @@
   </si>
   <si>
     <t>genus Chrysocromulina is only one - this maps to genus in FA - so this division in LTER matches to Genus in FA Chromulina</t>
+  </si>
+  <si>
+    <t>crypto - crypto</t>
+  </si>
+  <si>
+    <t>chloro - chloro</t>
+  </si>
+  <si>
+    <t>cyano cyano match</t>
+  </si>
+  <si>
+    <t>Ochryophya classes (Bac, Frag, Cosc) = diatoms</t>
+  </si>
+  <si>
+    <t>other can be average of everything else in PLoS paper</t>
   </si>
 </sst>
 </file>
@@ -496,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1032201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -5443,4 +5459,44 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>